<commit_message>
Published state of ETDataset on 8 January 2016
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/energy/energy_power_lv_network_electricity.xlsx
+++ b/nodes_source_analyses/energy/energy_power_lv_network_electricity.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="0" windowWidth="25600" windowHeight="16100" tabRatio="762"/>
+    <workbookView xWindow="1940" yWindow="0" windowWidth="25600" windowHeight="16100" tabRatio="762" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="93">
   <si>
     <t>Source</t>
   </si>
@@ -317,6 +317,9 @@
   </si>
   <si>
     <t>In order to get a realistic estimate of the available capacity on each of the voltage levels define in the ETM, each voltage level is described by a distribution of availabilities. The total capacity of the voltage is divided in 20 equal parts; for each part the average availability is defined as a percentage of the total capacity in that bin. These data are only used for the NL version of the ETM and stored in /etsource/datasets/nl/network.</t>
+  </si>
+  <si>
+    <t>Quintel assumption</t>
   </si>
 </sst>
 </file>
@@ -325,14 +328,21 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Lettertype hoofdtekst"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -759,390 +769,391 @@
   </borders>
   <cellStyleXfs count="260">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="10" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="11" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="260">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1919,7 +1930,7 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -2105,7 +2116,7 @@
   </sheetPr>
   <dimension ref="B1:K40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -2129,28 +2140,28 @@
       <c r="G1" s="22"/>
     </row>
     <row r="2" spans="2:11">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="90" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="68"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="92"/>
       <c r="F2" s="22"/>
       <c r="G2" s="22"/>
     </row>
     <row r="3" spans="2:11">
-      <c r="B3" s="69"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="71"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="95"/>
       <c r="F3" s="22"/>
       <c r="G3" s="22"/>
     </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="72"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="74"/>
+      <c r="B4" s="96"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="98"/>
       <c r="F4" s="22"/>
       <c r="G4" s="22"/>
     </row>
@@ -2227,7 +2238,7 @@
       <c r="F10" s="23"/>
       <c r="G10" s="23"/>
       <c r="H10" s="23"/>
-      <c r="I10" s="79" t="s">
+      <c r="I10" s="70" t="s">
         <v>85</v>
       </c>
       <c r="J10" s="62"/>
@@ -2247,7 +2258,7 @@
       <c r="F11" s="23"/>
       <c r="G11" s="23"/>
       <c r="H11" s="23"/>
-      <c r="I11" s="79" t="s">
+      <c r="I11" s="70" t="s">
         <v>85</v>
       </c>
       <c r="J11" s="62"/>
@@ -2255,7 +2266,7 @@
     </row>
     <row r="12" spans="2:11" ht="16" thickBot="1">
       <c r="B12" s="27"/>
-      <c r="C12" s="75" t="s">
+      <c r="C12" s="66" t="s">
         <v>77</v>
       </c>
       <c r="D12" s="13" t="s">
@@ -2267,7 +2278,7 @@
       <c r="F12" s="23"/>
       <c r="G12" s="23"/>
       <c r="H12" s="23"/>
-      <c r="I12" s="79" t="s">
+      <c r="I12" s="70" t="s">
         <v>85</v>
       </c>
       <c r="J12" s="62"/>
@@ -2287,7 +2298,7 @@
       <c r="F13" s="23"/>
       <c r="G13" s="23"/>
       <c r="H13" s="23"/>
-      <c r="I13" s="79" t="s">
+      <c r="I13" s="70" t="s">
         <v>85</v>
       </c>
       <c r="J13" s="62"/>
@@ -2307,7 +2318,7 @@
       <c r="F14" s="23"/>
       <c r="G14" s="23"/>
       <c r="H14" s="23"/>
-      <c r="I14" s="79" t="s">
+      <c r="I14" s="70" t="s">
         <v>85</v>
       </c>
       <c r="J14" s="62"/>
@@ -2329,7 +2340,7 @@
         <v>20</v>
       </c>
       <c r="H15" s="23"/>
-      <c r="I15" s="79" t="s">
+      <c r="I15" s="70" t="s">
         <v>85</v>
       </c>
       <c r="J15" s="62"/>
@@ -2350,7 +2361,7 @@
         <v>39</v>
       </c>
       <c r="H16" s="23"/>
-      <c r="I16" s="79" t="s">
+      <c r="I16" s="70" t="s">
         <v>85</v>
       </c>
       <c r="J16" s="62"/>
@@ -2369,7 +2380,7 @@
       <c r="F17" s="23"/>
       <c r="G17" s="23"/>
       <c r="H17" s="23"/>
-      <c r="I17" s="79" t="s">
+      <c r="I17" s="70" t="s">
         <v>86</v>
       </c>
       <c r="J17" s="62"/>
@@ -2388,7 +2399,7 @@
       <c r="F18" s="23"/>
       <c r="G18" s="23"/>
       <c r="H18" s="23"/>
-      <c r="I18" s="79" t="s">
+      <c r="I18" s="70" t="s">
         <v>86</v>
       </c>
       <c r="J18" s="62"/>
@@ -2407,7 +2418,7 @@
       <c r="F19" s="23"/>
       <c r="G19" s="23"/>
       <c r="H19" s="23"/>
-      <c r="I19" s="79" t="s">
+      <c r="I19" s="70" t="s">
         <v>85</v>
       </c>
       <c r="J19" s="62"/>
@@ -2421,15 +2432,15 @@
         <v>3</v>
       </c>
       <c r="E20" s="33">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="F20" s="23"/>
       <c r="G20" s="36" t="s">
         <v>50</v>
       </c>
       <c r="H20" s="23"/>
-      <c r="I20" s="79" t="s">
-        <v>85</v>
+      <c r="I20" s="99" t="s">
+        <v>92</v>
       </c>
       <c r="J20" s="62"/>
     </row>
@@ -2442,15 +2453,15 @@
         <v>3</v>
       </c>
       <c r="E21" s="33">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="F21" s="23"/>
       <c r="G21" s="36" t="s">
         <v>51</v>
       </c>
       <c r="H21" s="23"/>
-      <c r="I21" s="79" t="s">
-        <v>85</v>
+      <c r="I21" s="99" t="s">
+        <v>92</v>
       </c>
       <c r="J21" s="62"/>
     </row>
@@ -2463,15 +2474,15 @@
         <v>3</v>
       </c>
       <c r="E22" s="33">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="F22" s="23"/>
       <c r="G22" s="36" t="s">
         <v>52</v>
       </c>
       <c r="H22" s="23"/>
-      <c r="I22" s="79" t="s">
-        <v>85</v>
+      <c r="I22" s="99" t="s">
+        <v>92</v>
       </c>
       <c r="J22" s="62"/>
     </row>
@@ -2484,15 +2495,15 @@
         <v>3</v>
       </c>
       <c r="E23" s="33">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="F23" s="23"/>
       <c r="G23" s="36" t="s">
         <v>53</v>
       </c>
       <c r="H23" s="23"/>
-      <c r="I23" s="79" t="s">
-        <v>85</v>
+      <c r="I23" s="99" t="s">
+        <v>92</v>
       </c>
       <c r="J23" s="62"/>
     </row>
@@ -2512,7 +2523,7 @@
         <v>54</v>
       </c>
       <c r="H24" s="23"/>
-      <c r="I24" s="79" t="s">
+      <c r="I24" s="70" t="s">
         <v>85</v>
       </c>
       <c r="J24" s="62"/>
@@ -2557,7 +2568,7 @@
         <v>6</v>
       </c>
       <c r="H27" s="23"/>
-      <c r="I27" s="79" t="s">
+      <c r="I27" s="70" t="s">
         <v>85</v>
       </c>
       <c r="J27" s="62"/>
@@ -2578,7 +2589,7 @@
         <v>40</v>
       </c>
       <c r="H28" s="23"/>
-      <c r="I28" s="79" t="s">
+      <c r="I28" s="70" t="s">
         <v>85</v>
       </c>
       <c r="J28" s="62"/>
@@ -2599,7 +2610,7 @@
         <v>16</v>
       </c>
       <c r="H29" s="23"/>
-      <c r="I29" s="79" t="s">
+      <c r="I29" s="70" t="s">
         <v>85</v>
       </c>
       <c r="J29" s="62"/>
@@ -2620,7 +2631,7 @@
         <v>19</v>
       </c>
       <c r="H30" s="23"/>
-      <c r="I30" s="79" t="s">
+      <c r="I30" s="70" t="s">
         <v>85</v>
       </c>
       <c r="J30" s="62"/>
@@ -2641,7 +2652,7 @@
         <v>41</v>
       </c>
       <c r="H31" s="23"/>
-      <c r="I31" s="79" t="s">
+      <c r="I31" s="70" t="s">
         <v>85</v>
       </c>
       <c r="J31" s="62"/>
@@ -2662,7 +2673,7 @@
         <v>42</v>
       </c>
       <c r="H32" s="23"/>
-      <c r="I32" s="79" t="s">
+      <c r="I32" s="70" t="s">
         <v>85</v>
       </c>
       <c r="J32" s="62"/>
@@ -2683,7 +2694,7 @@
         <v>43</v>
       </c>
       <c r="H33" s="23"/>
-      <c r="I33" s="79" t="s">
+      <c r="I33" s="70" t="s">
         <v>85</v>
       </c>
       <c r="J33" s="62"/>
@@ -2696,7 +2707,7 @@
       <c r="D34" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E34" s="76">
+      <c r="E34" s="67">
         <v>5.5E-2</v>
       </c>
       <c r="F34" s="23"/>
@@ -2704,7 +2715,7 @@
         <v>15</v>
       </c>
       <c r="H34" s="23"/>
-      <c r="I34" s="79" t="s">
+      <c r="I34" s="70" t="s">
         <v>85</v>
       </c>
       <c r="J34" s="62"/>
@@ -2723,7 +2734,7 @@
       <c r="F35" s="23"/>
       <c r="G35" s="23"/>
       <c r="H35" s="23"/>
-      <c r="I35" s="79" t="s">
+      <c r="I35" s="70" t="s">
         <v>85</v>
       </c>
       <c r="J35" s="62"/>
@@ -2745,7 +2756,7 @@
         <v>5</v>
       </c>
       <c r="D37" s="57"/>
-      <c r="E37" s="77"/>
+      <c r="E37" s="68"/>
       <c r="F37" s="22"/>
       <c r="G37" s="22"/>
       <c r="H37" s="22"/>
@@ -2768,7 +2779,7 @@
         <v>18</v>
       </c>
       <c r="H38" s="23"/>
-      <c r="I38" s="80" t="s">
+      <c r="I38" s="71" t="s">
         <v>85</v>
       </c>
       <c r="J38" s="62"/>
@@ -2789,7 +2800,7 @@
         <v>17</v>
       </c>
       <c r="H39" s="23"/>
-      <c r="I39" s="80" t="s">
+      <c r="I39" s="71" t="s">
         <v>85</v>
       </c>
       <c r="J39" s="62"/>
@@ -2879,55 +2890,55 @@
       <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="90" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="68"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="92"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="B3" s="69"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="71"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="95"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="B4" s="69"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="71"/>
+      <c r="B4" s="93"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="95"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="B5" s="72"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="74"/>
+      <c r="B5" s="96"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="97"/>
+      <c r="H5" s="98"/>
     </row>
     <row r="6" spans="1:8">
       <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="65"/>
-      <c r="B7" s="83"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="87"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="78"/>
     </row>
     <row r="8" spans="1:8" ht="16" thickBot="1">
       <c r="A8" s="65"/>
@@ -2935,7 +2946,7 @@
       <c r="C8" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D8" s="81" t="s">
+      <c r="D8" s="72" t="s">
         <v>88</v>
       </c>
       <c r="E8" s="9" t="s">
@@ -2945,377 +2956,377 @@
       <c r="G8" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="H8" s="88"/>
+      <c r="H8" s="79"/>
     </row>
     <row r="9" spans="1:8" ht="16" thickBot="1">
       <c r="A9" s="65"/>
       <c r="B9" s="41"/>
-      <c r="C9" s="75">
+      <c r="C9" s="66">
         <v>1</v>
       </c>
-      <c r="D9" s="98">
+      <c r="D9" s="89">
         <v>5</v>
       </c>
-      <c r="E9" s="97">
+      <c r="E9" s="88">
         <v>0.53</v>
       </c>
-      <c r="F9" s="78"/>
-      <c r="G9" s="96" t="s">
+      <c r="F9" s="69"/>
+      <c r="G9" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="H9" s="88"/>
+      <c r="H9" s="79"/>
     </row>
     <row r="10" spans="1:8" ht="16" thickBot="1">
       <c r="A10" s="65"/>
       <c r="B10" s="41"/>
-      <c r="C10" s="75">
+      <c r="C10" s="66">
         <v>2</v>
       </c>
-      <c r="D10" s="98">
+      <c r="D10" s="89">
         <v>5</v>
       </c>
-      <c r="E10" s="97">
+      <c r="E10" s="88">
         <v>0.66</v>
       </c>
-      <c r="F10" s="78"/>
-      <c r="G10" s="96" t="s">
+      <c r="F10" s="69"/>
+      <c r="G10" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="H10" s="88"/>
+      <c r="H10" s="79"/>
     </row>
     <row r="11" spans="1:8" ht="16" thickBot="1">
       <c r="A11" s="65"/>
-      <c r="B11" s="89"/>
-      <c r="C11" s="75">
+      <c r="B11" s="80"/>
+      <c r="C11" s="66">
         <v>3</v>
       </c>
-      <c r="D11" s="98">
+      <c r="D11" s="89">
         <v>5</v>
       </c>
-      <c r="E11" s="97">
+      <c r="E11" s="88">
         <v>0.71</v>
       </c>
-      <c r="F11" s="78"/>
-      <c r="G11" s="96" t="s">
+      <c r="F11" s="69"/>
+      <c r="G11" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="H11" s="88"/>
+      <c r="H11" s="79"/>
     </row>
     <row r="12" spans="1:8" ht="16" thickBot="1">
       <c r="A12" s="65"/>
-      <c r="B12" s="89"/>
-      <c r="C12" s="75">
+      <c r="B12" s="80"/>
+      <c r="C12" s="66">
         <v>4</v>
       </c>
-      <c r="D12" s="98">
+      <c r="D12" s="89">
         <v>5</v>
       </c>
-      <c r="E12" s="97">
+      <c r="E12" s="88">
         <v>0.74</v>
       </c>
-      <c r="F12" s="78"/>
-      <c r="G12" s="96" t="s">
+      <c r="F12" s="69"/>
+      <c r="G12" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="H12" s="88"/>
+      <c r="H12" s="79"/>
     </row>
     <row r="13" spans="1:8" ht="16" thickBot="1">
       <c r="A13" s="65"/>
-      <c r="B13" s="89"/>
-      <c r="C13" s="75">
+      <c r="B13" s="80"/>
+      <c r="C13" s="66">
         <v>5</v>
       </c>
-      <c r="D13" s="98">
+      <c r="D13" s="89">
         <v>5</v>
       </c>
-      <c r="E13" s="97">
+      <c r="E13" s="88">
         <v>0.77</v>
       </c>
-      <c r="F13" s="78"/>
-      <c r="G13" s="96" t="s">
+      <c r="F13" s="69"/>
+      <c r="G13" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="H13" s="88"/>
+      <c r="H13" s="79"/>
     </row>
     <row r="14" spans="1:8" ht="16" thickBot="1">
       <c r="A14" s="65"/>
-      <c r="B14" s="89"/>
-      <c r="C14" s="75">
+      <c r="B14" s="80"/>
+      <c r="C14" s="66">
         <v>6</v>
       </c>
-      <c r="D14" s="98">
+      <c r="D14" s="89">
         <v>5</v>
       </c>
-      <c r="E14" s="97">
+      <c r="E14" s="88">
         <v>0.79</v>
       </c>
-      <c r="F14" s="78"/>
-      <c r="G14" s="96" t="s">
+      <c r="F14" s="69"/>
+      <c r="G14" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="H14" s="88"/>
+      <c r="H14" s="79"/>
     </row>
     <row r="15" spans="1:8" ht="16" thickBot="1">
       <c r="A15" s="65"/>
-      <c r="B15" s="89"/>
-      <c r="C15" s="75">
+      <c r="B15" s="80"/>
+      <c r="C15" s="66">
         <v>7</v>
       </c>
-      <c r="D15" s="98">
+      <c r="D15" s="89">
         <v>5</v>
       </c>
-      <c r="E15" s="97">
+      <c r="E15" s="88">
         <v>0.81</v>
       </c>
-      <c r="F15" s="78"/>
-      <c r="G15" s="96" t="s">
+      <c r="F15" s="69"/>
+      <c r="G15" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="H15" s="88"/>
+      <c r="H15" s="79"/>
     </row>
     <row r="16" spans="1:8" ht="16" thickBot="1">
       <c r="A16" s="65"/>
-      <c r="B16" s="89"/>
-      <c r="C16" s="75">
+      <c r="B16" s="80"/>
+      <c r="C16" s="66">
         <v>8</v>
       </c>
-      <c r="D16" s="98">
+      <c r="D16" s="89">
         <v>5</v>
       </c>
-      <c r="E16" s="97">
+      <c r="E16" s="88">
         <v>0.83</v>
       </c>
-      <c r="F16" s="78"/>
-      <c r="G16" s="96" t="s">
+      <c r="F16" s="69"/>
+      <c r="G16" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="H16" s="88"/>
+      <c r="H16" s="79"/>
     </row>
     <row r="17" spans="1:8" ht="16" thickBot="1">
       <c r="A17" s="65"/>
-      <c r="B17" s="89"/>
-      <c r="C17" s="75">
+      <c r="B17" s="80"/>
+      <c r="C17" s="66">
         <v>9</v>
       </c>
-      <c r="D17" s="98">
+      <c r="D17" s="89">
         <v>5</v>
       </c>
-      <c r="E17" s="97">
+      <c r="E17" s="88">
         <v>0.84</v>
       </c>
-      <c r="F17" s="78"/>
-      <c r="G17" s="96" t="s">
+      <c r="F17" s="69"/>
+      <c r="G17" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="H17" s="88"/>
+      <c r="H17" s="79"/>
     </row>
     <row r="18" spans="1:8" ht="16" thickBot="1">
       <c r="A18" s="65"/>
-      <c r="B18" s="89"/>
-      <c r="C18" s="75">
+      <c r="B18" s="80"/>
+      <c r="C18" s="66">
         <v>10</v>
       </c>
-      <c r="D18" s="98">
+      <c r="D18" s="89">
         <v>5</v>
       </c>
-      <c r="E18" s="97">
+      <c r="E18" s="88">
         <v>0.86</v>
       </c>
-      <c r="F18" s="78"/>
-      <c r="G18" s="96" t="s">
+      <c r="F18" s="69"/>
+      <c r="G18" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="H18" s="88"/>
+      <c r="H18" s="79"/>
     </row>
     <row r="19" spans="1:8" ht="16" thickBot="1">
       <c r="A19" s="65"/>
-      <c r="B19" s="89"/>
-      <c r="C19" s="75">
+      <c r="B19" s="80"/>
+      <c r="C19" s="66">
         <v>11</v>
       </c>
-      <c r="D19" s="98">
+      <c r="D19" s="89">
         <v>5</v>
       </c>
-      <c r="E19" s="97">
+      <c r="E19" s="88">
         <v>0.87</v>
       </c>
-      <c r="F19" s="78"/>
-      <c r="G19" s="96" t="s">
+      <c r="F19" s="69"/>
+      <c r="G19" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="H19" s="88"/>
+      <c r="H19" s="79"/>
     </row>
     <row r="20" spans="1:8" ht="16" thickBot="1">
       <c r="A20" s="65"/>
-      <c r="B20" s="89"/>
-      <c r="C20" s="75">
+      <c r="B20" s="80"/>
+      <c r="C20" s="66">
         <v>12</v>
       </c>
-      <c r="D20" s="98">
+      <c r="D20" s="89">
         <v>5</v>
       </c>
-      <c r="E20" s="97">
+      <c r="E20" s="88">
         <v>0.88</v>
       </c>
-      <c r="F20" s="78"/>
-      <c r="G20" s="96" t="s">
+      <c r="F20" s="69"/>
+      <c r="G20" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="H20" s="88"/>
+      <c r="H20" s="79"/>
     </row>
     <row r="21" spans="1:8" ht="16" thickBot="1">
       <c r="A21" s="65"/>
-      <c r="B21" s="89"/>
-      <c r="C21" s="75">
+      <c r="B21" s="80"/>
+      <c r="C21" s="66">
         <v>13</v>
       </c>
-      <c r="D21" s="98">
+      <c r="D21" s="89">
         <v>5</v>
       </c>
-      <c r="E21" s="97">
+      <c r="E21" s="88">
         <v>0.9</v>
       </c>
-      <c r="F21" s="78"/>
-      <c r="G21" s="96" t="s">
+      <c r="F21" s="69"/>
+      <c r="G21" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="H21" s="88"/>
+      <c r="H21" s="79"/>
     </row>
     <row r="22" spans="1:8" ht="16" thickBot="1">
       <c r="A22" s="65"/>
-      <c r="B22" s="89"/>
-      <c r="C22" s="75">
+      <c r="B22" s="80"/>
+      <c r="C22" s="66">
         <v>14</v>
       </c>
-      <c r="D22" s="98">
+      <c r="D22" s="89">
         <v>5</v>
       </c>
-      <c r="E22" s="97">
+      <c r="E22" s="88">
         <v>0.91</v>
       </c>
-      <c r="F22" s="78"/>
-      <c r="G22" s="96" t="s">
+      <c r="F22" s="69"/>
+      <c r="G22" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="H22" s="88"/>
+      <c r="H22" s="79"/>
     </row>
     <row r="23" spans="1:8" ht="16" thickBot="1">
       <c r="A23" s="65"/>
-      <c r="B23" s="89"/>
-      <c r="C23" s="75">
+      <c r="B23" s="80"/>
+      <c r="C23" s="66">
         <v>15</v>
       </c>
-      <c r="D23" s="98">
+      <c r="D23" s="89">
         <v>5</v>
       </c>
-      <c r="E23" s="97">
+      <c r="E23" s="88">
         <v>0.92</v>
       </c>
-      <c r="F23" s="78"/>
-      <c r="G23" s="96" t="s">
+      <c r="F23" s="69"/>
+      <c r="G23" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="H23" s="88"/>
+      <c r="H23" s="79"/>
     </row>
     <row r="24" spans="1:8" ht="16" thickBot="1">
       <c r="A24" s="65"/>
-      <c r="B24" s="89"/>
-      <c r="C24" s="75">
+      <c r="B24" s="80"/>
+      <c r="C24" s="66">
         <v>16</v>
       </c>
-      <c r="D24" s="98">
+      <c r="D24" s="89">
         <v>5</v>
       </c>
-      <c r="E24" s="97">
+      <c r="E24" s="88">
         <v>0.93</v>
       </c>
-      <c r="F24" s="78"/>
-      <c r="G24" s="96" t="s">
+      <c r="F24" s="69"/>
+      <c r="G24" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="H24" s="88"/>
+      <c r="H24" s="79"/>
     </row>
     <row r="25" spans="1:8" ht="16" thickBot="1">
       <c r="A25" s="65"/>
-      <c r="B25" s="89"/>
-      <c r="C25" s="75">
+      <c r="B25" s="80"/>
+      <c r="C25" s="66">
         <v>17</v>
       </c>
-      <c r="D25" s="98">
+      <c r="D25" s="89">
         <v>5</v>
       </c>
-      <c r="E25" s="97">
+      <c r="E25" s="88">
         <v>0.95</v>
       </c>
-      <c r="F25" s="78"/>
-      <c r="G25" s="96" t="s">
+      <c r="F25" s="69"/>
+      <c r="G25" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="H25" s="88"/>
+      <c r="H25" s="79"/>
     </row>
     <row r="26" spans="1:8" ht="16" thickBot="1">
       <c r="A26" s="65"/>
-      <c r="B26" s="89"/>
-      <c r="C26" s="75">
+      <c r="B26" s="80"/>
+      <c r="C26" s="66">
         <v>18</v>
       </c>
-      <c r="D26" s="98">
+      <c r="D26" s="89">
         <v>5</v>
       </c>
-      <c r="E26" s="97">
+      <c r="E26" s="88">
         <v>0.96</v>
       </c>
-      <c r="F26" s="78"/>
-      <c r="G26" s="96" t="s">
+      <c r="F26" s="69"/>
+      <c r="G26" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="H26" s="88"/>
+      <c r="H26" s="79"/>
     </row>
     <row r="27" spans="1:8" ht="16" thickBot="1">
       <c r="A27" s="65"/>
-      <c r="B27" s="89"/>
-      <c r="C27" s="75">
+      <c r="B27" s="80"/>
+      <c r="C27" s="66">
         <v>19</v>
       </c>
-      <c r="D27" s="98">
+      <c r="D27" s="89">
         <v>5</v>
       </c>
-      <c r="E27" s="97">
+      <c r="E27" s="88">
         <v>0.97</v>
       </c>
-      <c r="F27" s="78"/>
-      <c r="G27" s="96" t="s">
+      <c r="F27" s="69"/>
+      <c r="G27" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="H27" s="88"/>
+      <c r="H27" s="79"/>
     </row>
     <row r="28" spans="1:8" ht="16" thickBot="1">
       <c r="A28" s="65"/>
-      <c r="B28" s="89"/>
-      <c r="C28" s="75">
+      <c r="B28" s="80"/>
+      <c r="C28" s="66">
         <v>20</v>
       </c>
-      <c r="D28" s="98">
+      <c r="D28" s="89">
         <v>5</v>
       </c>
-      <c r="E28" s="97">
+      <c r="E28" s="88">
         <v>0.99</v>
       </c>
-      <c r="F28" s="78"/>
-      <c r="G28" s="96" t="s">
+      <c r="F28" s="69"/>
+      <c r="G28" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="H28" s="88"/>
+      <c r="H28" s="79"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="65"/>
-      <c r="B29" s="90"/>
-      <c r="C29" s="91"/>
-      <c r="D29" s="92"/>
-      <c r="E29" s="93"/>
-      <c r="F29" s="91"/>
-      <c r="G29" s="94"/>
-      <c r="H29" s="95"/>
+      <c r="B29" s="81"/>
+      <c r="C29" s="82"/>
+      <c r="D29" s="83"/>
+      <c r="E29" s="84"/>
+      <c r="F29" s="82"/>
+      <c r="G29" s="85"/>
+      <c r="H29" s="86"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="65"/>
@@ -3367,7 +3378,7 @@
       <c r="B35" s="22"/>
       <c r="C35" s="22"/>
       <c r="D35" s="57"/>
-      <c r="E35" s="82"/>
+      <c r="E35" s="73"/>
       <c r="F35" s="22"/>
       <c r="G35" s="65"/>
     </row>

</xml_diff>